<commit_message>
save 06 08 2025
</commit_message>
<xml_diff>
--- a/4 четверть_10_JavaScript_MoleculerJS.xlsx
+++ b/4 четверть_10_JavaScript_MoleculerJS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexServHW\Desktop\GB_Developer_Workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16983BA-C750-4B6A-8320-C10F01CBEEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6872640A-89D6-4051-92CD-4DDC74232279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9270" yWindow="-17490" windowWidth="23010" windowHeight="12210" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9270" yWindow="-20565" windowWidth="23010" windowHeight="18915" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="12" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1575" uniqueCount="1297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1595" uniqueCount="1315">
   <si>
     <t>Документация https://moleculer.services/docs/0.14/broker</t>
   </si>
@@ -12789,185 +12789,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Timeout
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Критически важный параметр!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Зачем нужен timeout в Moleculer.js?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Предотвращение "вечного ожидания"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Если сервис не отвечает (из-за ошибки, перегрузки или сетевых проблем), timeout гарантирует, что запрос не будет висеть бесконечно.
-После истечения таймаута вызывается ошибка (</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="4" tint="0.59999389629810485"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>RequestTimeoutError</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">), которую можно обработать.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Балансировка нагрузки и failover</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Moleculer может автоматически перенаправлять запросы к другому экземпляру сервиса, если текущий не ответил вовремя (благодаря встроенному механизму повторов и балансировки).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Защита от каскадных сбоев</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Без таймаута "зависший" сервис может вызвать цепочку проблем в других сервисах (например, исчерпание соединений или памяти).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Гибкость настройки</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Таймаут можно задавать:
-1 Глобально (в настройках брокера).
-2 На уровне действия (action) сервиса.
-3 Динамически при вызове (broker.call("service.action", {}, { timeout: 5000 })).</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <b/>
         <sz val="11"/>
@@ -13654,10 +13475,6 @@
     <t>Custom Error creation</t>
   </si>
   <si>
-    <t>`https://moleculer.services/docs/0.14/errors
-Продолжить</t>
-  </si>
-  <si>
     <t>Пользователь делает запрос (например, HTTP-запрос к API Gateway).</t>
   </si>
   <si>
@@ -13706,11 +13523,6 @@
   </si>
   <si>
     <t>return {Object}</t>
-  </si>
-  <si>
-    <t>`https://github.com/icebob/fastest-validator?tab=readme-ov-file#usage
-Продолжить
-service actions</t>
   </si>
   <si>
     <r>
@@ -14791,17 +14603,235 @@
   <si>
     <t>Interface</t>
   </si>
+  <si>
+    <t>`https://moleculer.services/docs/0.14/errors</t>
+  </si>
+  <si>
+    <r>
+      <t>Смотри</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> xls sheet - Controller (MoleculerError) </t>
+    </r>
+  </si>
+  <si>
+    <t>Если валидация параметров в action handler Moleculer.js провалена, фреймворк автоматически генерирует ошибку ValidationError (наследник MoleculerServerError), и дальнейшая обработка действия прерывается.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Если валидация параметров в action handler Moleculer.js </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>провалена</t>
+    </r>
+  </si>
+  <si>
+    <t>Структура ошибки</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: "ValidationError",
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>code</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: 422 (Unprocessable Entity),
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: "VALIDATION_ERROR",
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> — массив с описанием ошибок для каждого поля.</t>
+    </r>
+  </si>
+  <si>
+    <t>Автоматическая проверка параметров</t>
+  </si>
+  <si>
+    <t>Moleculer.js проверяет ctx.params перед вызовом handler. Если параметры не соответствуют схеме:
+1 Генерируется ошибка ValidationError (код 422 или 400).
+2 Действие не выполняется (handler не вызывается).</t>
+  </si>
+  <si>
+    <t>Пример тела ошибки:
+{
+  "name": "ValidationError",
+  "message": "Parameters validation error!",
+  "code": 422,
+  "type": "VALIDATION_ERROR",
+  "data": [
+    {
+      "field": "name",
+      "message": "The 'name' field must be a string with a minimum length of 3 characters."
+    },
+    {
+      "field": "age",
+      "message": "The 'age' field must be a positive number."
+    }
+  ]
+}</t>
+  </si>
+  <si>
+    <t>Гибкость настройки</t>
+  </si>
+  <si>
+    <t>Балансировка нагрузки и failover</t>
+  </si>
+  <si>
+    <t>Moleculer может автоматически перенаправлять запросы к другому экземпляру сервиса, если текущий не ответил вовремя (благодаря встроенному механизму повторов и балансировки).</t>
+  </si>
+  <si>
+    <t>Таймаут можно задавать:
+1 Глобально (в настройках брокера).
+2 На уровне действия (action) сервиса.
+3 Динамически при вызове (broker.call("service.action", {}, { timeout: 5000 })).</t>
+  </si>
+  <si>
+    <t>После истечения таймаута вызывается ошибка (RequestTimeoutError), которую можно обработать.</t>
+  </si>
+  <si>
+    <t>Предотвращение "вечного ожидания"</t>
+  </si>
+  <si>
+    <t>Если сервис не отвечает (из-за ошибки, перегрузки или сетевых проблем), timeout гарантирует, что запрос не будет висеть бесконечно.</t>
+  </si>
+  <si>
+    <t>Поведение на клиенте</t>
+  </si>
+  <si>
+    <t>1 Если действие вызывается через broker.call, ошибка передаётся как reject Promise.
+2 В API Gateway она преобразуется в HTTP-ответ с кодом 422 и JSON-телом (как выше).</t>
+  </si>
+  <si>
+    <t>Строгий режим валидации</t>
+  </si>
+  <si>
+    <t>params: {
+  $$strict: false, // Разрешить дополнительные поля
+  name: "string"
+}</t>
+  </si>
+  <si>
+    <t>По умолчанию Moleculer выбрасывает ошибку при любых лишних полях. Чтобы разрешить:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="36">
+  <fonts count="37">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -15076,8 +15106,9 @@
     </font>
     <font>
       <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="4" tint="0.59999389629810485"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -15085,9 +15116,8 @@
     </font>
     <font>
       <b/>
-      <u/>
       <sz val="11"/>
-      <color rgb="FFC00000"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -15400,23 +15430,23 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -15434,7 +15464,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -15452,7 +15482,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -15473,7 +15503,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -15494,7 +15524,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -15512,10 +15542,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -15524,28 +15554,28 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -15554,49 +15584,49 @@
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="23" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="23" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -15605,7 +15635,7 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -15614,7 +15644,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -15626,7 +15656,7 @@
     <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -15635,22 +15665,22 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -15662,73 +15692,73 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -16932,8 +16962,8 @@
   </sheetPr>
   <dimension ref="A2:V27"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -17073,7 +17103,7 @@
     </row>
     <row r="11" spans="1:22" ht="28.8">
       <c r="A11" s="45" t="s">
-        <v>1192</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="12" spans="1:22">
@@ -17082,7 +17112,7 @@
         <v>591</v>
       </c>
       <c r="C12" s="95" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="28.8">
@@ -17091,7 +17121,7 @@
         <v>592</v>
       </c>
       <c r="C13" s="95" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="14" spans="1:22">
@@ -17100,14 +17130,14 @@
         <v>593</v>
       </c>
       <c r="C14" s="95" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="72">
       <c r="A15" s="2"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>1191</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="43.2">
@@ -17116,75 +17146,78 @@
         <v>594</v>
       </c>
       <c r="C16" s="95" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="12" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="C17" s="95"/>
     </row>
     <row r="18" spans="1:4" ht="57.6">
       <c r="A18" s="2" t="s">
-        <v>1176</v>
-      </c>
-      <c r="C18" s="112" t="s">
-        <v>1196</v>
+        <v>1175</v>
+      </c>
+      <c r="C18" s="111" t="s">
+        <v>1193</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="72">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="C19" s="95" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="72">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="100.8">
       <c r="A21" s="2" t="s">
-        <v>1185</v>
-      </c>
-      <c r="C21" s="112" t="s">
-        <v>1197</v>
-      </c>
-      <c r="D21" s="108" t="s">
-        <v>1186</v>
+        <v>1184</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1295</v>
+      </c>
+      <c r="C21" s="111" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>1294</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="43.2">
       <c r="A22" s="95" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>843</v>
       </c>
       <c r="C22" s="95" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="43.2">
       <c r="B23" s="95" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="C23" s="95" t="s">
+        <v>1178</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>1179</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>1180</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -17193,7 +17226,7 @@
         <v>953</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -17204,13 +17237,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="57.6">
-      <c r="D27" s="108" t="s">
-        <v>1195</v>
-      </c>
+    <row r="27" spans="1:4">
+      <c r="D27" s="4"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="13" type="noConversion"/>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="10" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -17321,7 +17352,7 @@
       <c r="A5" s="2"/>
       <c r="B5" s="1"/>
       <c r="C5" s="66" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D5" s="2"/>
       <c r="F5" s="1"/>
@@ -17470,7 +17501,7 @@
         <v>689</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="C11" s="52" t="s">
         <v>691</v>
@@ -17519,7 +17550,7 @@
     </row>
     <row r="13" spans="1:22" s="7" customFormat="1">
       <c r="A13" s="107" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="B13" s="49"/>
       <c r="C13" s="58"/>
@@ -17642,7 +17673,7 @@
     </row>
     <row r="18" spans="1:22" s="7" customFormat="1" ht="86.4">
       <c r="A18" s="107" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>512</v>
@@ -18077,7 +18108,7 @@
     </row>
     <row r="35" spans="1:22" s="7" customFormat="1">
       <c r="A35" s="107" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="B35" s="49"/>
       <c r="C35" s="58"/>
@@ -18453,10 +18484,10 @@
     </row>
     <row r="4" spans="1:22" ht="360">
       <c r="B4" s="2" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="C4" s="95" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="P4" s="1"/>
       <c r="U4" s="1"/>
@@ -18467,7 +18498,7 @@
         <v>934</v>
       </c>
       <c r="B5" s="64" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="C5" s="95" t="s">
         <v>866</v>
@@ -20989,12 +21020,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC501503-0164-402D-9D9C-86B5F52AE94D}">
   <sheetPr>
+    <tabColor theme="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:V69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -21048,11 +21080,11 @@
       <c r="U2" s="5"/>
     </row>
     <row r="3" spans="1:22">
-      <c r="C3" s="113" t="s">
-        <v>1198</v>
+      <c r="C3" s="112" t="s">
+        <v>1195</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1199</v>
+        <v>1196</v>
       </c>
       <c r="P3" s="1"/>
       <c r="U3" s="1"/>
@@ -21060,7 +21092,7 @@
     </row>
     <row r="4" spans="1:22" s="7" customFormat="1">
       <c r="A4" s="12" t="s">
-        <v>1198</v>
+        <v>1195</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="4"/>
@@ -21083,11 +21115,11 @@
     </row>
     <row r="5" spans="1:22" s="7" customFormat="1" ht="115.2">
       <c r="A5" s="1" t="s">
-        <v>1222</v>
+        <v>1219</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>1212</v>
+        <v>1209</v>
       </c>
       <c r="D5" s="1"/>
       <c r="F5" s="1"/>
@@ -21137,14 +21169,14 @@
     </row>
     <row r="7" spans="1:22" s="7" customFormat="1">
       <c r="A7" s="1" t="s">
-        <v>1201</v>
+        <v>1198</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="1" t="s">
-        <v>1202</v>
+        <v>1199</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="2"/>
@@ -21164,16 +21196,16 @@
     </row>
     <row r="8" spans="1:22" s="7" customFormat="1">
       <c r="A8" s="1" t="s">
-        <v>1203</v>
+        <v>1200</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>84</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>1210</v>
+        <v>1207</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="2"/>
@@ -21193,14 +21225,14 @@
     </row>
     <row r="9" spans="1:22" s="7" customFormat="1">
       <c r="A9" s="1" t="s">
-        <v>1205</v>
+        <v>1202</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="1" t="s">
-        <v>1206</v>
+        <v>1203</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="2"/>
@@ -21220,14 +21252,14 @@
     </row>
     <row r="10" spans="1:22" s="7" customFormat="1">
       <c r="A10" s="1" t="s">
-        <v>1207</v>
+        <v>1204</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>1208</v>
+        <v>1205</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="1" t="s">
-        <v>1209</v>
+        <v>1206</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="2"/>
@@ -21265,11 +21297,11 @@
       <c r="U11" s="5"/>
     </row>
     <row r="12" spans="1:22">
-      <c r="C12" s="113" t="s">
-        <v>1200</v>
+      <c r="C12" s="112" t="s">
+        <v>1197</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>1223</v>
+        <v>1220</v>
       </c>
       <c r="P12" s="1"/>
       <c r="U12" s="1"/>
@@ -21277,7 +21309,7 @@
     </row>
     <row r="13" spans="1:22" s="7" customFormat="1">
       <c r="A13" s="12" t="s">
-        <v>1200</v>
+        <v>1197</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -21300,56 +21332,56 @@
     </row>
     <row r="14" spans="1:22" ht="57.6">
       <c r="B14" s="2" t="s">
-        <v>1225</v>
-      </c>
-      <c r="C14" s="112" t="s">
-        <v>1213</v>
+        <v>1222</v>
+      </c>
+      <c r="C14" s="111" t="s">
+        <v>1210</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="201.6">
       <c r="B15" s="2" t="s">
-        <v>1214</v>
-      </c>
-      <c r="C15" s="112" t="s">
-        <v>1216</v>
+        <v>1211</v>
+      </c>
+      <c r="C15" s="111" t="s">
+        <v>1213</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="43.2">
       <c r="B16" s="2" t="s">
-        <v>1215</v>
-      </c>
-      <c r="C16" s="112" t="s">
-        <v>1217</v>
+        <v>1212</v>
+      </c>
+      <c r="C16" s="111" t="s">
+        <v>1214</v>
       </c>
     </row>
     <row r="17" spans="1:22">
       <c r="A17" s="1" t="s">
-        <v>1218</v>
-      </c>
-      <c r="C17" s="112"/>
+        <v>1215</v>
+      </c>
+      <c r="C17" s="111"/>
     </row>
     <row r="18" spans="1:22" ht="144">
-      <c r="C18" s="112" t="s">
-        <v>1220</v>
+      <c r="C18" s="111" t="s">
+        <v>1217</v>
       </c>
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="1" t="s">
-        <v>1219</v>
-      </c>
-      <c r="C19" s="112"/>
+        <v>1216</v>
+      </c>
+      <c r="C19" s="111"/>
     </row>
     <row r="20" spans="1:22" ht="244.8">
-      <c r="C20" s="112" t="s">
-        <v>1221</v>
+      <c r="C20" s="111" t="s">
+        <v>1218</v>
       </c>
     </row>
     <row r="21" spans="1:22" ht="115.2">
       <c r="A21" s="1" t="s">
-        <v>1222</v>
-      </c>
-      <c r="C21" s="112" t="s">
-        <v>1211</v>
+        <v>1219</v>
+      </c>
+      <c r="C21" s="111" t="s">
+        <v>1208</v>
       </c>
     </row>
     <row r="22" spans="1:22">
@@ -21359,7 +21391,7 @@
       <c r="B22" s="57" t="s">
         <v>305</v>
       </c>
-      <c r="C22" s="114" t="s">
+      <c r="C22" s="113" t="s">
         <v>306</v>
       </c>
       <c r="D22" s="55" t="s">
@@ -21368,49 +21400,49 @@
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="1" t="s">
-        <v>1201</v>
+        <v>1198</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>1202</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="1" t="s">
-        <v>1203</v>
+        <v>1200</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>84</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>1210</v>
+        <v>1207</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="25" spans="1:22">
       <c r="A25" s="1" t="s">
-        <v>1205</v>
+        <v>1202</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>1206</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="26" spans="1:22">
       <c r="A26" s="1" t="s">
-        <v>1207</v>
+        <v>1204</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>1208</v>
+        <v>1205</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>1209</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="28" spans="1:22">
@@ -21433,8 +21465,8 @@
       <c r="U28" s="5"/>
     </row>
     <row r="29" spans="1:22">
-      <c r="C29" s="113" t="s">
-        <v>1226</v>
+      <c r="C29" s="112" t="s">
+        <v>1223</v>
       </c>
       <c r="P29" s="1"/>
       <c r="U29" s="1"/>
@@ -21442,7 +21474,7 @@
     </row>
     <row r="30" spans="1:22" ht="28.8">
       <c r="C30" s="2" t="s">
-        <v>1228</v>
+        <v>1225</v>
       </c>
       <c r="P30" s="1"/>
       <c r="U30" s="1"/>
@@ -21450,28 +21482,28 @@
     </row>
     <row r="31" spans="1:22">
       <c r="A31" s="12" t="s">
-        <v>1224</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="32" spans="1:22">
-      <c r="C32" s="112" t="s">
-        <v>1231</v>
+      <c r="C32" s="111" t="s">
+        <v>1228</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>1230</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="33" spans="1:22">
       <c r="A33" s="12" t="s">
-        <v>1227</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="34" spans="1:22">
-      <c r="C34" s="112" t="s">
-        <v>1232</v>
+      <c r="C34" s="111" t="s">
+        <v>1229</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>1229</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="36" spans="1:22">
@@ -21494,11 +21526,11 @@
       <c r="U36" s="5"/>
     </row>
     <row r="37" spans="1:22">
-      <c r="C37" s="113" t="s">
-        <v>1233</v>
+      <c r="C37" s="112" t="s">
+        <v>1230</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>1234</v>
+        <v>1231</v>
       </c>
       <c r="P37" s="1"/>
       <c r="U37" s="1"/>
@@ -21506,145 +21538,145 @@
     </row>
     <row r="38" spans="1:22" ht="43.2">
       <c r="A38" s="1" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>1235</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>1238</v>
-      </c>
-      <c r="C38" s="112" t="s">
-        <v>1236</v>
+      <c r="C38" s="111" t="s">
+        <v>1233</v>
       </c>
     </row>
     <row r="39" spans="1:22" ht="43.2">
       <c r="A39" s="1" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C39" s="111" t="s">
         <v>1237</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>1239</v>
-      </c>
-      <c r="C39" s="112" t="s">
-        <v>1240</v>
       </c>
     </row>
     <row r="40" spans="1:22" ht="43.2">
       <c r="A40" s="1" t="s">
-        <v>1241</v>
+        <v>1238</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>1243</v>
-      </c>
-      <c r="C40" s="112" t="s">
-        <v>1242</v>
+        <v>1240</v>
+      </c>
+      <c r="C40" s="111" t="s">
+        <v>1239</v>
       </c>
     </row>
     <row r="41" spans="1:22" ht="43.2">
       <c r="A41" s="1" t="s">
-        <v>1244</v>
+        <v>1241</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>1246</v>
-      </c>
-      <c r="C41" s="112" t="s">
-        <v>1245</v>
+        <v>1243</v>
+      </c>
+      <c r="C41" s="111" t="s">
+        <v>1242</v>
       </c>
     </row>
     <row r="42" spans="1:22" ht="43.2">
       <c r="A42" s="1" t="s">
-        <v>1247</v>
+        <v>1244</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>1249</v>
-      </c>
-      <c r="C42" s="112" t="s">
-        <v>1248</v>
+        <v>1246</v>
+      </c>
+      <c r="C42" s="111" t="s">
+        <v>1245</v>
       </c>
     </row>
     <row r="43" spans="1:22" ht="43.2">
       <c r="A43" s="1" t="s">
-        <v>1250</v>
+        <v>1247</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>1252</v>
-      </c>
-      <c r="C43" s="112" t="s">
-        <v>1251</v>
+        <v>1249</v>
+      </c>
+      <c r="C43" s="111" t="s">
+        <v>1248</v>
       </c>
     </row>
     <row r="44" spans="1:22" ht="43.2">
       <c r="A44" s="1" t="s">
-        <v>1253</v>
+        <v>1250</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>1255</v>
-      </c>
-      <c r="C44" s="112" t="s">
-        <v>1254</v>
+        <v>1252</v>
+      </c>
+      <c r="C44" s="111" t="s">
+        <v>1251</v>
       </c>
     </row>
     <row r="45" spans="1:22" ht="43.2">
       <c r="A45" s="1" t="s">
-        <v>1256</v>
+        <v>1253</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>1258</v>
-      </c>
-      <c r="C45" s="112" t="s">
-        <v>1257</v>
+        <v>1255</v>
+      </c>
+      <c r="C45" s="111" t="s">
+        <v>1254</v>
       </c>
     </row>
     <row r="46" spans="1:22" ht="43.2">
       <c r="A46" s="1" t="s">
-        <v>1259</v>
+        <v>1256</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>1261</v>
-      </c>
-      <c r="C46" s="112" t="s">
-        <v>1260</v>
+        <v>1258</v>
+      </c>
+      <c r="C46" s="111" t="s">
+        <v>1257</v>
       </c>
     </row>
     <row r="47" spans="1:22" ht="43.2">
       <c r="A47" s="1" t="s">
-        <v>1262</v>
+        <v>1259</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>1264</v>
-      </c>
-      <c r="C47" s="112" t="s">
-        <v>1263</v>
+        <v>1261</v>
+      </c>
+      <c r="C47" s="111" t="s">
+        <v>1260</v>
       </c>
     </row>
     <row r="48" spans="1:22" ht="43.2">
       <c r="A48" s="1" t="s">
-        <v>1265</v>
+        <v>1262</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>1267</v>
-      </c>
-      <c r="C48" s="112" t="s">
-        <v>1266</v>
+        <v>1264</v>
+      </c>
+      <c r="C48" s="111" t="s">
+        <v>1263</v>
       </c>
     </row>
     <row r="49" spans="1:22" ht="43.2">
       <c r="A49" s="1" t="s">
-        <v>1268</v>
+        <v>1265</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>1270</v>
-      </c>
-      <c r="C49" s="112" t="s">
-        <v>1269</v>
+        <v>1267</v>
+      </c>
+      <c r="C49" s="111" t="s">
+        <v>1266</v>
       </c>
     </row>
     <row r="50" spans="1:22" ht="43.2">
       <c r="A50" s="1" t="s">
-        <v>1271</v>
+        <v>1268</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>1273</v>
-      </c>
-      <c r="C50" s="112" t="s">
-        <v>1272</v>
+        <v>1270</v>
+      </c>
+      <c r="C50" s="111" t="s">
+        <v>1269</v>
       </c>
     </row>
     <row r="52" spans="1:22">
@@ -21667,19 +21699,19 @@
       <c r="U52" s="5"/>
     </row>
     <row r="53" spans="1:22">
-      <c r="C53" s="113" t="s">
-        <v>1274</v>
+      <c r="C53" s="112" t="s">
+        <v>1271</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>1275</v>
+        <v>1272</v>
       </c>
       <c r="P53" s="1"/>
       <c r="U53" s="1"/>
       <c r="V53" s="2"/>
     </row>
     <row r="55" spans="1:22" ht="100.8">
-      <c r="C55" s="112" t="s">
-        <v>1197</v>
+      <c r="C55" s="111" t="s">
+        <v>1194</v>
       </c>
     </row>
     <row r="57" spans="1:22">
@@ -21702,11 +21734,11 @@
       <c r="U57" s="5"/>
     </row>
     <row r="58" spans="1:22">
-      <c r="C58" s="113" t="s">
-        <v>1276</v>
+      <c r="C58" s="112" t="s">
+        <v>1273</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>1277</v>
+        <v>1274</v>
       </c>
       <c r="P58" s="1"/>
       <c r="U58" s="1"/>
@@ -21717,54 +21749,54 @@
         <v>67</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>1296</v>
-      </c>
-      <c r="C59" s="112" t="s">
-        <v>1278</v>
+        <v>1293</v>
+      </c>
+      <c r="C59" s="111" t="s">
+        <v>1275</v>
       </c>
     </row>
     <row r="60" spans="1:22">
       <c r="A60" s="55" t="s">
-        <v>1279</v>
+        <v>1276</v>
       </c>
       <c r="B60" s="57" t="s">
-        <v>1280</v>
-      </c>
-      <c r="C60" s="114" t="s">
+        <v>1277</v>
+      </c>
+      <c r="C60" s="113" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="61" spans="1:22">
       <c r="A61" s="1" t="s">
-        <v>1281</v>
+        <v>1278</v>
       </c>
       <c r="B61" s="2" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C61" s="4" t="s">
         <v>1282</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>1285</v>
       </c>
     </row>
     <row r="62" spans="1:22">
       <c r="A62" s="1" t="s">
-        <v>1283</v>
+        <v>1280</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>1286</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="63" spans="1:22" ht="28.8">
       <c r="A63" s="1" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>1284</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>1287</v>
-      </c>
       <c r="C63" s="4" t="s">
-        <v>1288</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="64" spans="1:22">
@@ -21774,39 +21806,39 @@
     </row>
     <row r="65" spans="1:3" ht="129.6">
       <c r="A65" s="1" t="s">
-        <v>1282</v>
-      </c>
-      <c r="C65" s="112" t="s">
-        <v>1294</v>
+        <v>1279</v>
+      </c>
+      <c r="C65" s="111" t="s">
+        <v>1291</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="28.8">
       <c r="A66" s="90" t="s">
         <v>67</v>
       </c>
-      <c r="C66" s="112" t="s">
+      <c r="C66" s="111" t="s">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="115.2">
+      <c r="B67" s="111" t="s">
         <v>1289</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" ht="115.2">
-      <c r="B67" s="112" t="s">
+      <c r="C67" s="111" t="s">
         <v>1292</v>
       </c>
-      <c r="C67" s="112" t="s">
-        <v>1295</v>
-      </c>
     </row>
     <row r="68" spans="1:3" ht="100.8">
-      <c r="B68" s="112" t="s">
-        <v>1293</v>
-      </c>
-      <c r="C68" s="112" t="s">
-        <v>1291</v>
+      <c r="B68" s="111" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C68" s="111" t="s">
+        <v>1288</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="28.8">
-      <c r="C69" s="112" t="s">
-        <v>1290</v>
+      <c r="C69" s="111" t="s">
+        <v>1287</v>
       </c>
     </row>
   </sheetData>
@@ -23147,7 +23179,7 @@
         <v>124</v>
       </c>
       <c r="B64" s="64" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="D64" s="13" t="s">
         <v>125</v>
@@ -24506,10 +24538,10 @@
     <tabColor theme="5" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:V70"/>
+  <dimension ref="A2:V80"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -25082,7 +25114,7 @@
         <v>394</v>
       </c>
       <c r="C23" s="96" t="s">
-        <v>1194</v>
+        <v>1192</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>648</v>
@@ -25175,13 +25207,13 @@
       <c r="V26" s="1"/>
     </row>
     <row r="27" spans="1:22" s="7" customFormat="1" ht="43.2">
-      <c r="A27" s="110" t="s">
+      <c r="A27" s="109" t="s">
         <v>649</v>
       </c>
       <c r="B27" s="95" t="s">
-        <v>1193</v>
-      </c>
-      <c r="C27" s="111" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C27" s="110" t="s">
         <v>425</v>
       </c>
       <c r="D27" s="90"/>
@@ -25203,7 +25235,7 @@
     </row>
     <row r="28" spans="1:22" s="7" customFormat="1" ht="144">
       <c r="A28" s="95" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="B28" s="95" t="s">
         <v>457</v>
@@ -25230,10 +25262,10 @@
     </row>
     <row r="29" spans="1:22" s="7" customFormat="1" ht="230.4">
       <c r="A29" s="95" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>1169</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>1170</v>
       </c>
       <c r="C29" s="87" t="s">
         <v>850</v>
@@ -25257,13 +25289,17 @@
       <c r="U29" s="2"/>
       <c r="V29" s="1"/>
     </row>
-    <row r="30" spans="1:22" s="7" customFormat="1">
-      <c r="A30" s="62" t="s">
-        <v>1143</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="87"/>
-      <c r="D30" s="87"/>
+    <row r="30" spans="1:22" s="7" customFormat="1" ht="43.2">
+      <c r="A30" s="63" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B30" s="114" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C30" s="114" t="s">
+        <v>1296</v>
+      </c>
+      <c r="D30" s="52"/>
       <c r="F30" s="1"/>
       <c r="G30" s="2"/>
       <c r="H30" s="1"/>
@@ -25280,13 +25316,15 @@
       <c r="U30" s="2"/>
       <c r="V30" s="1"/>
     </row>
-    <row r="31" spans="1:22" s="7" customFormat="1" ht="216">
-      <c r="A31" s="52"/>
-      <c r="B31" s="2" t="s">
-        <v>1171</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>1146</v>
+    <row r="31" spans="1:22" s="7" customFormat="1" ht="57.6">
+      <c r="A31" s="114" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B31" s="114" t="s">
+        <v>1314</v>
+      </c>
+      <c r="C31" s="114" t="s">
+        <v>1313</v>
       </c>
       <c r="D31" s="52"/>
       <c r="F31" s="1"/>
@@ -25306,16 +25344,14 @@
       <c r="V31" s="1"/>
     </row>
     <row r="32" spans="1:22" s="7" customFormat="1" ht="72">
-      <c r="A32" s="1" t="s">
-        <v>1144</v>
+      <c r="A32" s="114" t="s">
+        <v>1300</v>
       </c>
       <c r="B32" s="2"/>
-      <c r="C32" s="95" t="s">
-        <v>1138</v>
-      </c>
-      <c r="D32" s="95" t="s">
-        <v>1139</v>
-      </c>
+      <c r="C32" s="114" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D32" s="52"/>
       <c r="F32" s="1"/>
       <c r="G32" s="2"/>
       <c r="H32" s="1"/>
@@ -25332,15 +25368,13 @@
       <c r="U32" s="2"/>
       <c r="V32" s="1"/>
     </row>
-    <row r="33" spans="1:22" s="7" customFormat="1" ht="259.2">
-      <c r="A33" s="1" t="s">
-        <v>1145</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>727</v>
-      </c>
-      <c r="C33" s="95" t="s">
-        <v>1140</v>
+    <row r="33" spans="1:22" s="7" customFormat="1" ht="57.6">
+      <c r="A33" s="114" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B33" s="87"/>
+      <c r="C33" s="114" t="s">
+        <v>1311</v>
       </c>
       <c r="D33" s="52"/>
       <c r="F33" s="1"/>
@@ -25359,18 +25393,16 @@
       <c r="U33" s="2"/>
       <c r="V33" s="1"/>
     </row>
-    <row r="34" spans="1:22" s="7" customFormat="1" ht="409.6">
-      <c r="A34" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="B34" s="66" t="s">
-        <v>1132</v>
-      </c>
-      <c r="C34" s="87" t="s">
-        <v>668</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>669</v>
+    <row r="34" spans="1:22" s="7" customFormat="1" ht="259.2">
+      <c r="A34" s="114" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="114" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D34" s="114" t="s">
+        <v>1302</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="2"/>
@@ -25389,18 +25421,12 @@
       <c r="V34" s="1"/>
     </row>
     <row r="35" spans="1:22" s="7" customFormat="1">
-      <c r="A35" s="12" t="s">
-        <v>427</v>
-      </c>
-      <c r="B35" s="100" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C35" s="109" t="s">
-        <v>884</v>
-      </c>
-      <c r="D35" s="90" t="s">
-        <v>651</v>
-      </c>
+      <c r="A35" s="62" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="87"/>
+      <c r="D35" s="87"/>
       <c r="F35" s="1"/>
       <c r="G35" s="2"/>
       <c r="H35" s="1"/>
@@ -25417,17 +25443,15 @@
       <c r="U35" s="2"/>
       <c r="V35" s="1"/>
     </row>
-    <row r="36" spans="1:22" s="7" customFormat="1" ht="144">
-      <c r="A36" s="1"/>
-      <c r="B36" s="52" t="s">
-        <v>650</v>
+    <row r="36" spans="1:22" s="7" customFormat="1" ht="216">
+      <c r="A36" s="52"/>
+      <c r="B36" s="2" t="s">
+        <v>1170</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="D36" s="52" t="s">
-        <v>429</v>
-      </c>
+        <v>1145</v>
+      </c>
+      <c r="D36" s="52"/>
       <c r="F36" s="1"/>
       <c r="G36" s="2"/>
       <c r="H36" s="1"/>
@@ -25444,13 +25468,17 @@
       <c r="U36" s="2"/>
       <c r="V36" s="1"/>
     </row>
-    <row r="37" spans="1:22" s="7" customFormat="1">
-      <c r="A37" s="47" t="s">
-        <v>1162</v>
-      </c>
-      <c r="B37" s="52"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="52"/>
+    <row r="37" spans="1:22" s="7" customFormat="1" ht="72">
+      <c r="A37" s="1" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="95" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D37" s="95" t="s">
+        <v>1138</v>
+      </c>
       <c r="F37" s="1"/>
       <c r="G37" s="2"/>
       <c r="H37" s="1"/>
@@ -25467,17 +25495,17 @@
       <c r="U37" s="2"/>
       <c r="V37" s="1"/>
     </row>
-    <row r="38" spans="1:22" s="7" customFormat="1">
+    <row r="38" spans="1:22" s="7" customFormat="1" ht="259.2">
       <c r="A38" s="1" t="s">
-        <v>1152</v>
-      </c>
-      <c r="B38" s="2"/>
+        <v>1144</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>727</v>
+      </c>
       <c r="C38" s="95" t="s">
-        <v>1157</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>652</v>
-      </c>
+        <v>1139</v>
+      </c>
+      <c r="D38" s="52"/>
       <c r="F38" s="1"/>
       <c r="G38" s="2"/>
       <c r="H38" s="1"/>
@@ -25495,14 +25523,12 @@
       <c r="V38" s="1"/>
     </row>
     <row r="39" spans="1:22" s="7" customFormat="1">
-      <c r="A39" s="1" t="s">
-        <v>1153</v>
+      <c r="A39" s="13" t="s">
+        <v>478</v>
       </c>
       <c r="B39" s="2"/>
-      <c r="C39" s="95" t="s">
-        <v>1154</v>
-      </c>
-      <c r="D39" s="1"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
       <c r="F39" s="1"/>
       <c r="G39" s="2"/>
       <c r="H39" s="1"/>
@@ -25519,15 +25545,15 @@
       <c r="U39" s="2"/>
       <c r="V39" s="1"/>
     </row>
-    <row r="40" spans="1:22" s="7" customFormat="1" ht="72">
-      <c r="A40" s="1" t="s">
-        <v>1155</v>
-      </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="95" t="s">
-        <v>1156</v>
-      </c>
-      <c r="D40" s="1"/>
+    <row r="40" spans="1:22" s="7" customFormat="1" ht="316.8">
+      <c r="A40" s="87"/>
+      <c r="B40" s="87"/>
+      <c r="C40" s="87" t="s">
+        <v>668</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>669</v>
+      </c>
       <c r="F40" s="1"/>
       <c r="G40" s="2"/>
       <c r="H40" s="1"/>
@@ -25544,15 +25570,15 @@
       <c r="U40" s="2"/>
       <c r="V40" s="1"/>
     </row>
-    <row r="41" spans="1:22" s="7" customFormat="1" ht="43.2">
-      <c r="A41" s="1" t="s">
-        <v>1158</v>
-      </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="95" t="s">
-        <v>1159</v>
-      </c>
-      <c r="D41" s="1"/>
+    <row r="41" spans="1:22" s="7" customFormat="1" ht="28.8">
+      <c r="A41" s="50" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B41" s="87"/>
+      <c r="C41" s="114" t="s">
+        <v>1307</v>
+      </c>
+      <c r="D41" s="2"/>
       <c r="F41" s="1"/>
       <c r="G41" s="2"/>
       <c r="H41" s="1"/>
@@ -25569,15 +25595,15 @@
       <c r="U41" s="2"/>
       <c r="V41" s="1"/>
     </row>
-    <row r="42" spans="1:22" s="7" customFormat="1">
-      <c r="A42" s="1" t="s">
-        <v>1160</v>
-      </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="95" t="s">
-        <v>1161</v>
-      </c>
-      <c r="D42" s="1"/>
+    <row r="42" spans="1:22" s="7" customFormat="1" ht="28.8">
+      <c r="A42" s="114" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B42" s="87"/>
+      <c r="C42" s="114" t="s">
+        <v>1309</v>
+      </c>
+      <c r="D42" s="2"/>
       <c r="F42" s="1"/>
       <c r="G42" s="2"/>
       <c r="H42" s="1"/>
@@ -25594,15 +25620,15 @@
       <c r="U42" s="2"/>
       <c r="V42" s="1"/>
     </row>
-    <row r="43" spans="1:22" s="7" customFormat="1">
-      <c r="A43" s="47" t="s">
-        <v>1163</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>1164</v>
-      </c>
-      <c r="C43" s="95"/>
-      <c r="D43" s="1"/>
+    <row r="43" spans="1:22" s="7" customFormat="1" ht="43.2">
+      <c r="A43" s="1" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B43" s="87"/>
+      <c r="C43" s="114" t="s">
+        <v>1305</v>
+      </c>
+      <c r="D43" s="2"/>
       <c r="F43" s="1"/>
       <c r="G43" s="2"/>
       <c r="H43" s="1"/>
@@ -25619,20 +25645,16 @@
       <c r="U43" s="2"/>
       <c r="V43" s="1"/>
     </row>
-    <row r="44" spans="1:22" s="7" customFormat="1">
-      <c r="A44" s="55" t="s">
-        <v>304</v>
-      </c>
-      <c r="B44" s="57" t="s">
-        <v>305</v>
-      </c>
-      <c r="C44" s="55" t="s">
-        <v>307</v>
-      </c>
-      <c r="D44" s="56" t="s">
-        <v>306</v>
-      </c>
-      <c r="F44" s="2"/>
+    <row r="44" spans="1:22" s="7" customFormat="1" ht="57.6">
+      <c r="A44" s="1" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B44" s="87"/>
+      <c r="C44" s="114" t="s">
+        <v>1306</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="F44" s="1"/>
       <c r="G44" s="2"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -25648,20 +25670,20 @@
       <c r="U44" s="2"/>
       <c r="V44" s="1"/>
     </row>
-    <row r="45" spans="1:22" s="7" customFormat="1" ht="57.6">
-      <c r="A45" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>852</v>
-      </c>
-      <c r="C45" s="66" t="s">
-        <v>664</v>
-      </c>
-      <c r="D45" s="87" t="s">
-        <v>856</v>
-      </c>
-      <c r="F45" s="2"/>
+    <row r="45" spans="1:22" s="7" customFormat="1">
+      <c r="A45" s="12" t="s">
+        <v>427</v>
+      </c>
+      <c r="B45" s="100" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C45" s="108" t="s">
+        <v>884</v>
+      </c>
+      <c r="D45" s="90" t="s">
+        <v>651</v>
+      </c>
+      <c r="F45" s="1"/>
       <c r="G45" s="2"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -25677,20 +25699,18 @@
       <c r="U45" s="2"/>
       <c r="V45" s="1"/>
     </row>
-    <row r="46" spans="1:22" s="7" customFormat="1" ht="57.6">
-      <c r="A46" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>853</v>
-      </c>
-      <c r="C46" s="66" t="s">
-        <v>663</v>
-      </c>
-      <c r="D46" s="87" t="s">
-        <v>857</v>
-      </c>
-      <c r="F46" s="2"/>
+    <row r="46" spans="1:22" s="7" customFormat="1" ht="144">
+      <c r="A46" s="1"/>
+      <c r="B46" s="52" t="s">
+        <v>650</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D46" s="52" t="s">
+        <v>429</v>
+      </c>
+      <c r="F46" s="1"/>
       <c r="G46" s="2"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
@@ -25706,20 +25726,14 @@
       <c r="U46" s="2"/>
       <c r="V46" s="1"/>
     </row>
-    <row r="47" spans="1:22" s="7" customFormat="1" ht="158.4">
-      <c r="A47" s="1" t="s">
-        <v>654</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>854</v>
-      </c>
-      <c r="C47" s="64" t="s">
-        <v>662</v>
-      </c>
-      <c r="D47" s="87" t="s">
-        <v>855</v>
-      </c>
-      <c r="F47" s="2"/>
+    <row r="47" spans="1:22" s="7" customFormat="1">
+      <c r="A47" s="47" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B47" s="52"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="52"/>
+      <c r="F47" s="1"/>
       <c r="G47" s="2"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
@@ -25737,18 +25751,16 @@
     </row>
     <row r="48" spans="1:22" s="7" customFormat="1">
       <c r="A48" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>655</v>
-      </c>
-      <c r="D48" s="52" t="s">
-        <v>546</v>
-      </c>
-      <c r="F48" s="2"/>
+        <v>1151</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" s="95" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="F48" s="1"/>
       <c r="G48" s="2"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
@@ -25764,20 +25776,16 @@
       <c r="U48" s="2"/>
       <c r="V48" s="1"/>
     </row>
-    <row r="49" spans="1:22" s="7" customFormat="1" ht="43.2">
+    <row r="49" spans="1:22" s="7" customFormat="1">
       <c r="A49" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>667</v>
-      </c>
-      <c r="C49" s="64" t="s">
-        <v>666</v>
-      </c>
-      <c r="D49" s="52" t="s">
-        <v>657</v>
-      </c>
-      <c r="F49" s="2"/>
+        <v>1152</v>
+      </c>
+      <c r="B49" s="2"/>
+      <c r="C49" s="95" t="s">
+        <v>1153</v>
+      </c>
+      <c r="D49" s="1"/>
+      <c r="F49" s="1"/>
       <c r="G49" s="2"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
@@ -25793,20 +25801,16 @@
       <c r="U49" s="2"/>
       <c r="V49" s="1"/>
     </row>
-    <row r="50" spans="1:22" s="7" customFormat="1">
+    <row r="50" spans="1:22" s="7" customFormat="1" ht="72">
       <c r="A50" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>514</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>659</v>
-      </c>
-      <c r="D50" s="52" t="s">
-        <v>546</v>
-      </c>
-      <c r="F50" s="2"/>
+        <v>1154</v>
+      </c>
+      <c r="B50" s="2"/>
+      <c r="C50" s="95" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D50" s="1"/>
+      <c r="F50" s="1"/>
       <c r="G50" s="2"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -25822,20 +25826,16 @@
       <c r="U50" s="2"/>
       <c r="V50" s="1"/>
     </row>
-    <row r="51" spans="1:22" s="7" customFormat="1">
+    <row r="51" spans="1:22" s="7" customFormat="1" ht="43.2">
       <c r="A51" s="1" t="s">
-        <v>660</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>661</v>
-      </c>
-      <c r="D51" s="52" t="s">
-        <v>546</v>
-      </c>
-      <c r="F51" s="2"/>
+        <v>1157</v>
+      </c>
+      <c r="B51" s="2"/>
+      <c r="C51" s="95" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D51" s="1"/>
+      <c r="F51" s="1"/>
       <c r="G51" s="2"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
@@ -25852,17 +25852,15 @@
       <c r="V51" s="1"/>
     </row>
     <row r="52" spans="1:22" s="7" customFormat="1">
-      <c r="A52" s="12" t="s">
-        <v>886</v>
-      </c>
-      <c r="B52" s="100" t="s">
-        <v>1166</v>
-      </c>
-      <c r="C52" s="90" t="s">
-        <v>670</v>
-      </c>
-      <c r="D52" s="111"/>
-      <c r="F52" s="2"/>
+      <c r="A52" s="1" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B52" s="2"/>
+      <c r="C52" s="95" t="s">
+        <v>1160</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="F52" s="1"/>
       <c r="G52" s="2"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
@@ -25878,18 +25876,16 @@
       <c r="U52" s="2"/>
       <c r="V52" s="1"/>
     </row>
-    <row r="53" spans="1:22" s="7" customFormat="1" ht="158.4">
-      <c r="A53" s="66" t="s">
-        <v>675</v>
+    <row r="53" spans="1:22" s="7" customFormat="1">
+      <c r="A53" s="47" t="s">
+        <v>1162</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>672</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>674</v>
-      </c>
-      <c r="D53" s="52"/>
-      <c r="F53" s="2"/>
+        <v>1163</v>
+      </c>
+      <c r="C53" s="95"/>
+      <c r="D53" s="1"/>
+      <c r="F53" s="1"/>
       <c r="G53" s="2"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
@@ -25905,15 +25901,19 @@
       <c r="U53" s="2"/>
       <c r="V53" s="1"/>
     </row>
-    <row r="54" spans="1:22" s="7" customFormat="1" ht="158.4">
-      <c r="A54" s="1"/>
-      <c r="B54" s="2" t="s">
-        <v>671</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>673</v>
-      </c>
-      <c r="D54" s="52"/>
+    <row r="54" spans="1:22" s="7" customFormat="1">
+      <c r="A54" s="55" t="s">
+        <v>304</v>
+      </c>
+      <c r="B54" s="57" t="s">
+        <v>305</v>
+      </c>
+      <c r="C54" s="55" t="s">
+        <v>307</v>
+      </c>
+      <c r="D54" s="56" t="s">
+        <v>306</v>
+      </c>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="1"/>
@@ -25930,13 +25930,19 @@
       <c r="U54" s="2"/>
       <c r="V54" s="1"/>
     </row>
-    <row r="55" spans="1:22" s="7" customFormat="1">
+    <row r="55" spans="1:22" s="7" customFormat="1" ht="57.6">
       <c r="A55" s="1" t="s">
-        <v>677</v>
-      </c>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="52"/>
+        <v>478</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>852</v>
+      </c>
+      <c r="C55" s="66" t="s">
+        <v>664</v>
+      </c>
+      <c r="D55" s="87" t="s">
+        <v>856</v>
+      </c>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
       <c r="H55" s="1"/>
@@ -25953,16 +25959,18 @@
       <c r="U55" s="2"/>
       <c r="V55" s="1"/>
     </row>
-    <row r="56" spans="1:22" s="7" customFormat="1" ht="172.8">
-      <c r="A56" s="1"/>
+    <row r="56" spans="1:22" s="7" customFormat="1" ht="57.6">
+      <c r="A56" s="1" t="s">
+        <v>653</v>
+      </c>
       <c r="B56" s="2" t="s">
-        <v>676</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>679</v>
-      </c>
-      <c r="D56" s="52" t="s">
-        <v>678</v>
+        <v>853</v>
+      </c>
+      <c r="C56" s="66" t="s">
+        <v>663</v>
+      </c>
+      <c r="D56" s="87" t="s">
+        <v>857</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
@@ -25980,17 +25988,19 @@
       <c r="U56" s="2"/>
       <c r="V56" s="1"/>
     </row>
-    <row r="57" spans="1:22" s="7" customFormat="1">
-      <c r="A57" s="12" t="s">
-        <v>428</v>
-      </c>
-      <c r="B57" s="100" t="s">
-        <v>1167</v>
-      </c>
-      <c r="C57" s="109" t="s">
-        <v>883</v>
-      </c>
-      <c r="D57" s="111"/>
+    <row r="57" spans="1:22" s="7" customFormat="1" ht="158.4">
+      <c r="A57" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>854</v>
+      </c>
+      <c r="C57" s="64" t="s">
+        <v>662</v>
+      </c>
+      <c r="D57" s="87" t="s">
+        <v>855</v>
+      </c>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
       <c r="H57" s="1"/>
@@ -26007,16 +26017,20 @@
       <c r="U57" s="2"/>
       <c r="V57" s="1"/>
     </row>
-    <row r="58" spans="1:22" s="7" customFormat="1" ht="259.2">
-      <c r="A58" s="2"/>
-      <c r="B58" s="52" t="s">
-        <v>665</v>
-      </c>
-      <c r="C58" s="52" t="s">
-        <v>432</v>
-      </c>
-      <c r="D58" s="1"/>
-      <c r="F58" s="1"/>
+    <row r="58" spans="1:22" s="7" customFormat="1">
+      <c r="A58" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="D58" s="52" t="s">
+        <v>546</v>
+      </c>
+      <c r="F58" s="2"/>
       <c r="G58" s="2"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
@@ -26032,14 +26046,20 @@
       <c r="U58" s="2"/>
       <c r="V58" s="1"/>
     </row>
-    <row r="59" spans="1:22" s="7" customFormat="1">
-      <c r="A59" s="1"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="52" t="s">
-        <v>431</v>
-      </c>
-      <c r="D59" s="1"/>
-      <c r="F59" s="1"/>
+    <row r="59" spans="1:22" s="7" customFormat="1" ht="43.2">
+      <c r="A59" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>667</v>
+      </c>
+      <c r="C59" s="64" t="s">
+        <v>666</v>
+      </c>
+      <c r="D59" s="52" t="s">
+        <v>657</v>
+      </c>
+      <c r="F59" s="2"/>
       <c r="G59" s="2"/>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
@@ -26055,18 +26075,20 @@
       <c r="U59" s="2"/>
       <c r="V59" s="1"/>
     </row>
-    <row r="60" spans="1:22" s="7" customFormat="1" ht="43.2">
-      <c r="A60" s="1"/>
+    <row r="60" spans="1:22" s="7" customFormat="1">
+      <c r="A60" s="1" t="s">
+        <v>658</v>
+      </c>
       <c r="B60" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="C60" s="52" t="s">
-        <v>434</v>
+        <v>514</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>659</v>
       </c>
       <c r="D60" s="52" t="s">
-        <v>435</v>
-      </c>
-      <c r="F60" s="1"/>
+        <v>546</v>
+      </c>
+      <c r="F60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
@@ -26083,13 +26105,19 @@
       <c r="V60" s="1"/>
     </row>
     <row r="61" spans="1:22" s="7" customFormat="1">
-      <c r="A61" s="12" t="s">
-        <v>762</v>
-      </c>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="52"/>
-      <c r="F61" s="1"/>
+      <c r="A61" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="D61" s="52" t="s">
+        <v>546</v>
+      </c>
+      <c r="F61" s="2"/>
       <c r="G61" s="2"/>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
@@ -26105,14 +26133,18 @@
       <c r="U61" s="2"/>
       <c r="V61" s="1"/>
     </row>
-    <row r="62" spans="1:22" s="7" customFormat="1" ht="273.60000000000002">
-      <c r="A62" s="1"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2" t="s">
-        <v>885</v>
-      </c>
-      <c r="D62" s="52"/>
-      <c r="F62" s="1"/>
+    <row r="62" spans="1:22" s="7" customFormat="1">
+      <c r="A62" s="12" t="s">
+        <v>886</v>
+      </c>
+      <c r="B62" s="100" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C62" s="90" t="s">
+        <v>670</v>
+      </c>
+      <c r="D62" s="110"/>
+      <c r="F62" s="2"/>
       <c r="G62" s="2"/>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
@@ -26128,18 +26160,18 @@
       <c r="U62" s="2"/>
       <c r="V62" s="1"/>
     </row>
-    <row r="63" spans="1:22" s="7" customFormat="1">
-      <c r="A63" s="12" t="s">
-        <v>332</v>
-      </c>
-      <c r="B63" s="45" t="s">
-        <v>393</v>
-      </c>
-      <c r="C63" s="60"/>
-      <c r="D63" s="12" t="s">
-        <v>448</v>
-      </c>
-      <c r="F63" s="1"/>
+    <row r="63" spans="1:22" s="7" customFormat="1" ht="158.4">
+      <c r="A63" s="66" t="s">
+        <v>675</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>672</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="D63" s="52"/>
+      <c r="F63" s="2"/>
       <c r="G63" s="2"/>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
@@ -26155,14 +26187,16 @@
       <c r="U63" s="2"/>
       <c r="V63" s="1"/>
     </row>
-    <row r="64" spans="1:22" s="7" customFormat="1" ht="43.2">
-      <c r="A64" s="2"/>
-      <c r="B64" s="2"/>
-      <c r="C64" s="52" t="s">
-        <v>447</v>
-      </c>
-      <c r="D64" s="1"/>
-      <c r="F64" s="1"/>
+    <row r="64" spans="1:22" s="7" customFormat="1" ht="158.4">
+      <c r="A64" s="1"/>
+      <c r="B64" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="D64" s="52"/>
+      <c r="F64" s="2"/>
       <c r="G64" s="2"/>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
@@ -26179,15 +26213,13 @@
       <c r="V64" s="1"/>
     </row>
     <row r="65" spans="1:22" s="7" customFormat="1">
-      <c r="A65" s="49" t="s">
-        <v>455</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="C65" s="52"/>
-      <c r="D65" s="1"/>
-      <c r="F65" s="1"/>
+      <c r="A65" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="52"/>
+      <c r="F65" s="2"/>
       <c r="G65" s="2"/>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
@@ -26203,14 +26235,18 @@
       <c r="U65" s="2"/>
       <c r="V65" s="1"/>
     </row>
-    <row r="66" spans="1:22" s="7" customFormat="1" ht="288">
-      <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="52" t="s">
-        <v>449</v>
-      </c>
-      <c r="D66" s="1"/>
-      <c r="F66" s="1"/>
+    <row r="66" spans="1:22" s="7" customFormat="1" ht="172.8">
+      <c r="A66" s="1"/>
+      <c r="B66" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="D66" s="52" t="s">
+        <v>678</v>
+      </c>
+      <c r="F66" s="2"/>
       <c r="G66" s="2"/>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
@@ -26226,16 +26262,18 @@
       <c r="U66" s="2"/>
       <c r="V66" s="1"/>
     </row>
-    <row r="67" spans="1:22" s="7" customFormat="1" ht="43.2">
-      <c r="A67" s="49" t="s">
-        <v>456</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>895</v>
-      </c>
-      <c r="C67" s="52"/>
-      <c r="D67" s="1"/>
-      <c r="F67" s="1"/>
+    <row r="67" spans="1:22" s="7" customFormat="1">
+      <c r="A67" s="12" t="s">
+        <v>428</v>
+      </c>
+      <c r="B67" s="100" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C67" s="108" t="s">
+        <v>883</v>
+      </c>
+      <c r="D67" s="110"/>
+      <c r="F67" s="2"/>
       <c r="G67" s="2"/>
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
@@ -26251,13 +26289,13 @@
       <c r="U67" s="2"/>
       <c r="V67" s="1"/>
     </row>
-    <row r="68" spans="1:22" s="7" customFormat="1" ht="187.2">
-      <c r="A68" s="93"/>
-      <c r="B68" s="2" t="s">
-        <v>887</v>
-      </c>
-      <c r="C68" s="93" t="s">
-        <v>450</v>
+    <row r="68" spans="1:22" s="7" customFormat="1" ht="259.2">
+      <c r="A68" s="2"/>
+      <c r="B68" s="52" t="s">
+        <v>665</v>
+      </c>
+      <c r="C68" s="52" t="s">
+        <v>432</v>
       </c>
       <c r="D68" s="1"/>
       <c r="F68" s="1"/>
@@ -26277,16 +26315,12 @@
       <c r="V68" s="1"/>
     </row>
     <row r="69" spans="1:22" s="7" customFormat="1">
-      <c r="A69" s="2" t="s">
-        <v>451</v>
-      </c>
-      <c r="B69" s="52" t="s">
-        <v>453</v>
-      </c>
-      <c r="C69" s="2"/>
-      <c r="D69" s="1" t="s">
-        <v>452</v>
-      </c>
+      <c r="A69" s="1"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="52" t="s">
+        <v>431</v>
+      </c>
+      <c r="D69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="2"/>
       <c r="H69" s="1"/>
@@ -26303,13 +26337,17 @@
       <c r="U69" s="2"/>
       <c r="V69" s="1"/>
     </row>
-    <row r="70" spans="1:22" s="7" customFormat="1" ht="172.8">
-      <c r="A70" s="2"/>
-      <c r="B70" s="2"/>
-      <c r="C70" s="93" t="s">
-        <v>454</v>
-      </c>
-      <c r="D70" s="1"/>
+    <row r="70" spans="1:22" s="7" customFormat="1" ht="43.2">
+      <c r="A70" s="1"/>
+      <c r="B70" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C70" s="52" t="s">
+        <v>434</v>
+      </c>
+      <c r="D70" s="52" t="s">
+        <v>435</v>
+      </c>
       <c r="F70" s="1"/>
       <c r="G70" s="2"/>
       <c r="H70" s="1"/>
@@ -26325,6 +26363,250 @@
       <c r="T70" s="8"/>
       <c r="U70" s="2"/>
       <c r="V70" s="1"/>
+    </row>
+    <row r="71" spans="1:22" s="7" customFormat="1">
+      <c r="A71" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="52"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="2"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="K71" s="1"/>
+      <c r="L71" s="1"/>
+      <c r="M71" s="1"/>
+      <c r="N71" s="1"/>
+      <c r="P71" s="2"/>
+      <c r="Q71" s="2"/>
+      <c r="R71" s="2"/>
+      <c r="S71" s="1"/>
+      <c r="T71" s="8"/>
+      <c r="U71" s="2"/>
+      <c r="V71" s="1"/>
+    </row>
+    <row r="72" spans="1:22" s="7" customFormat="1" ht="273.60000000000002">
+      <c r="A72" s="1"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2" t="s">
+        <v>885</v>
+      </c>
+      <c r="D72" s="52"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+      <c r="K72" s="1"/>
+      <c r="L72" s="1"/>
+      <c r="M72" s="1"/>
+      <c r="N72" s="1"/>
+      <c r="P72" s="2"/>
+      <c r="Q72" s="2"/>
+      <c r="R72" s="2"/>
+      <c r="S72" s="1"/>
+      <c r="T72" s="8"/>
+      <c r="U72" s="2"/>
+      <c r="V72" s="1"/>
+    </row>
+    <row r="73" spans="1:22" s="7" customFormat="1">
+      <c r="A73" s="12" t="s">
+        <v>332</v>
+      </c>
+      <c r="B73" s="45" t="s">
+        <v>393</v>
+      </c>
+      <c r="C73" s="60"/>
+      <c r="D73" s="12" t="s">
+        <v>448</v>
+      </c>
+      <c r="F73" s="1"/>
+      <c r="G73" s="2"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="K73" s="1"/>
+      <c r="L73" s="1"/>
+      <c r="M73" s="1"/>
+      <c r="N73" s="1"/>
+      <c r="P73" s="2"/>
+      <c r="Q73" s="2"/>
+      <c r="R73" s="2"/>
+      <c r="S73" s="1"/>
+      <c r="T73" s="8"/>
+      <c r="U73" s="2"/>
+      <c r="V73" s="1"/>
+    </row>
+    <row r="74" spans="1:22" s="7" customFormat="1" ht="43.2">
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="52" t="s">
+        <v>447</v>
+      </c>
+      <c r="D74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="2"/>
+      <c r="H74" s="1"/>
+      <c r="I74" s="1"/>
+      <c r="K74" s="1"/>
+      <c r="L74" s="1"/>
+      <c r="M74" s="1"/>
+      <c r="N74" s="1"/>
+      <c r="P74" s="2"/>
+      <c r="Q74" s="2"/>
+      <c r="R74" s="2"/>
+      <c r="S74" s="1"/>
+      <c r="T74" s="8"/>
+      <c r="U74" s="2"/>
+      <c r="V74" s="1"/>
+    </row>
+    <row r="75" spans="1:22" s="7" customFormat="1">
+      <c r="A75" s="49" t="s">
+        <v>455</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="C75" s="52"/>
+      <c r="D75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="K75" s="1"/>
+      <c r="L75" s="1"/>
+      <c r="M75" s="1"/>
+      <c r="N75" s="1"/>
+      <c r="P75" s="2"/>
+      <c r="Q75" s="2"/>
+      <c r="R75" s="2"/>
+      <c r="S75" s="1"/>
+      <c r="T75" s="8"/>
+      <c r="U75" s="2"/>
+      <c r="V75" s="1"/>
+    </row>
+    <row r="76" spans="1:22" s="7" customFormat="1" ht="288">
+      <c r="A76" s="2"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="52" t="s">
+        <v>449</v>
+      </c>
+      <c r="D76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="1"/>
+      <c r="I76" s="1"/>
+      <c r="K76" s="1"/>
+      <c r="L76" s="1"/>
+      <c r="M76" s="1"/>
+      <c r="N76" s="1"/>
+      <c r="P76" s="2"/>
+      <c r="Q76" s="2"/>
+      <c r="R76" s="2"/>
+      <c r="S76" s="1"/>
+      <c r="T76" s="8"/>
+      <c r="U76" s="2"/>
+      <c r="V76" s="1"/>
+    </row>
+    <row r="77" spans="1:22" s="7" customFormat="1" ht="43.2">
+      <c r="A77" s="49" t="s">
+        <v>456</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>895</v>
+      </c>
+      <c r="C77" s="52"/>
+      <c r="D77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="2"/>
+      <c r="H77" s="1"/>
+      <c r="I77" s="1"/>
+      <c r="K77" s="1"/>
+      <c r="L77" s="1"/>
+      <c r="M77" s="1"/>
+      <c r="N77" s="1"/>
+      <c r="P77" s="2"/>
+      <c r="Q77" s="2"/>
+      <c r="R77" s="2"/>
+      <c r="S77" s="1"/>
+      <c r="T77" s="8"/>
+      <c r="U77" s="2"/>
+      <c r="V77" s="1"/>
+    </row>
+    <row r="78" spans="1:22" s="7" customFormat="1" ht="187.2">
+      <c r="A78" s="93"/>
+      <c r="B78" s="2" t="s">
+        <v>887</v>
+      </c>
+      <c r="C78" s="93" t="s">
+        <v>450</v>
+      </c>
+      <c r="D78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="1"/>
+      <c r="I78" s="1"/>
+      <c r="K78" s="1"/>
+      <c r="L78" s="1"/>
+      <c r="M78" s="1"/>
+      <c r="N78" s="1"/>
+      <c r="P78" s="2"/>
+      <c r="Q78" s="2"/>
+      <c r="R78" s="2"/>
+      <c r="S78" s="1"/>
+      <c r="T78" s="8"/>
+      <c r="U78" s="2"/>
+      <c r="V78" s="1"/>
+    </row>
+    <row r="79" spans="1:22" s="7" customFormat="1">
+      <c r="A79" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="B79" s="52" t="s">
+        <v>453</v>
+      </c>
+      <c r="C79" s="2"/>
+      <c r="D79" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="F79" s="1"/>
+      <c r="G79" s="2"/>
+      <c r="H79" s="1"/>
+      <c r="I79" s="1"/>
+      <c r="K79" s="1"/>
+      <c r="L79" s="1"/>
+      <c r="M79" s="1"/>
+      <c r="N79" s="1"/>
+      <c r="P79" s="2"/>
+      <c r="Q79" s="2"/>
+      <c r="R79" s="2"/>
+      <c r="S79" s="1"/>
+      <c r="T79" s="8"/>
+      <c r="U79" s="2"/>
+      <c r="V79" s="1"/>
+    </row>
+    <row r="80" spans="1:22" s="7" customFormat="1" ht="172.8">
+      <c r="A80" s="2"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="93" t="s">
+        <v>454</v>
+      </c>
+      <c r="D80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="1"/>
+      <c r="I80" s="1"/>
+      <c r="K80" s="1"/>
+      <c r="L80" s="1"/>
+      <c r="M80" s="1"/>
+      <c r="N80" s="1"/>
+      <c r="P80" s="2"/>
+      <c r="Q80" s="2"/>
+      <c r="R80" s="2"/>
+      <c r="S80" s="1"/>
+      <c r="T80" s="8"/>
+      <c r="U80" s="2"/>
+      <c r="V80" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -27424,7 +27706,7 @@
     </row>
     <row r="16" spans="1:22" s="7" customFormat="1">
       <c r="A16" s="98" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="B16" s="90"/>
       <c r="C16" s="90"/>
@@ -27447,7 +27729,7 @@
     </row>
     <row r="17" spans="1:22" s="7" customFormat="1" ht="360">
       <c r="A17" s="2" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="B17" s="95" t="s">
         <v>457</v>
@@ -27476,16 +27758,16 @@
     </row>
     <row r="18" spans="1:22" s="7" customFormat="1" ht="288">
       <c r="A18" s="52" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="C18" s="59" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D18" s="59" t="s">
         <v>1148</v>
-      </c>
-      <c r="D18" s="59" t="s">
-        <v>1149</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="2"/>

</xml_diff>

<commit_message>
save 01 09 2025
</commit_message>
<xml_diff>
--- a/4 четверть_10_JavaScript_MoleculerJS.xlsx
+++ b/4 четверть_10_JavaScript_MoleculerJS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexServHW\Desktop\GB_Developer_Workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60E8718-049B-4E07-97B2-43A569C2D21C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F726B8-09FD-4CF4-B953-F218B772E70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6525" yWindow="-21165" windowWidth="23010" windowHeight="17460" firstSheet="16" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="13" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="12" r:id="rId1"/>
@@ -49,12 +49,15 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1817" uniqueCount="1516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1818" uniqueCount="1517">
   <si>
     <t>Документация https://moleculer.services/docs/0.14/broker</t>
   </si>
@@ -14967,69 +14970,6 @@
     <t>Мой любимый вариант, так как можно дополнительно указать middlewares</t>
   </si>
   <si>
-    <r>
-      <t>broker.createService({
-    mixins: [ApiService],
-    settings: {
-        routes: [{
-            aliases: {
-                "POST upload"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(req, res) {
-                    this.parseUploadedFile(req, res);
-                },</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-                "GET custom"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(req, res) {
-                    res.end('hello from custom handler')
-                }</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-            }
-        }]
-    }
-});</t>
-    </r>
-  </si>
-  <si>
     <t>req.$ctx</t>
   </si>
   <si>
@@ -15559,27 +15499,6 @@
   </si>
   <si>
     <t>`https://moleculer.services/docs/0.14/moleculer-web#Auto-alias</t>
-  </si>
-  <si>
-    <t>// api.service.js
-module.exports = {
-    mixins: [ApiGateway],
-    settings: {
-        routes: [
-            {
-                path: "/api",
-                whitelist: [
-                    "v2.posts.*",
-                    "test.*"
-                ],
-                aliases: {
-                    "GET /hi": "test.hello"
-                },
-                autoAliases: true
-            }
-        ]
-    }
-};</t>
   </si>
   <si>
     <t>GET     /api/hi             =&gt; test.hello
@@ -17219,17 +17138,161 @@
 3 Дополнительные middleware: Можно использовать любые Express middleware перед moleculer-web
 4 Легаси-интеграция: Постепенная миграция с Express на Moleculer</t>
   </si>
+  <si>
+    <t>Modify responce in action
+Redirection</t>
+  </si>
+  <si>
+    <r>
+      <t>broker.createService({
+    mixins: [ApiService],
+    settings: {
+        routes: [{
+            aliases: {
+                "POST upload"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(req, res) {
+                    this.parseUploadedFile(req, res); </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>//action name</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+                },</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+                "GET custom"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(req, res) {
+                    res.end('hello from custom handler')
+                }</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+            }
+        }]
+    }
+});</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">// api.service.js
+module.exports = {
+    mixins: [ApiGateway],
+    settings: {
+        routes: [
+            {
+                path: "/api",
+                whitelist: [
+                    "v2.posts.*",
+                    "test.*"
+                ],
+                aliases: {
+                    "GET /hi": "test.hello"
+                },
+               </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> autoAliases: true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+            }
+        ]
+    }
+};</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="40">
+  <fonts count="41">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -17850,7 +17913,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -17861,23 +17924,23 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -17895,7 +17958,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -17913,7 +17976,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -17934,7 +17997,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -17955,7 +18018,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -17973,10 +18036,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -17985,28 +18048,28 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="23" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -18015,49 +18078,49 @@
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="23" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="23" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -18066,7 +18129,7 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -18075,7 +18138,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -18087,7 +18150,7 @@
     <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -18096,22 +18159,22 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -18123,89 +18186,92 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="22" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="24" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="25" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -19687,7 +19753,7 @@
       <c r="D27" s="4"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="15" type="noConversion"/>
+  <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="10" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -22916,8 +22982,8 @@
   </sheetPr>
   <dimension ref="A2:V87"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -22989,7 +23055,7 @@
         <v>350</v>
       </c>
       <c r="B4" s="115" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>351</v>
@@ -23582,7 +23648,7 @@
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="2"/>
@@ -23746,10 +23812,10 @@
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="49" t="s">
-        <v>1430</v>
+        <v>1428</v>
       </c>
       <c r="D36" s="49" t="s">
-        <v>1429</v>
+        <v>1427</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="2"/>
@@ -23773,10 +23839,10 @@
         <v>1349</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>1350</v>
+        <v>1515</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>1431</v>
+        <v>1429</v>
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="2"/>
@@ -23796,11 +23862,11 @@
     </row>
     <row r="38" spans="1:22" s="7" customFormat="1">
       <c r="A38" s="102" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
-        <v>1369</v>
+        <v>1368</v>
       </c>
       <c r="D38" s="2"/>
       <c r="F38" s="1"/>
@@ -23821,11 +23887,11 @@
     </row>
     <row r="39" spans="1:22" s="7" customFormat="1">
       <c r="A39" s="2" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="D39" s="2"/>
       <c r="F39" s="1"/>
@@ -23846,11 +23912,11 @@
     </row>
     <row r="40" spans="1:22" s="7" customFormat="1">
       <c r="A40" s="2" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="D40" s="2"/>
       <c r="F40" s="1"/>
@@ -23871,11 +23937,11 @@
     </row>
     <row r="41" spans="1:22" s="7" customFormat="1">
       <c r="A41" s="2" t="s">
-        <v>1356</v>
+        <v>1355</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
-        <v>1355</v>
+        <v>1354</v>
       </c>
       <c r="D41" s="2"/>
       <c r="F41" s="1"/>
@@ -23896,11 +23962,11 @@
     </row>
     <row r="42" spans="1:22" s="7" customFormat="1">
       <c r="A42" s="2" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="D42" s="2"/>
       <c r="F42" s="1"/>
@@ -23921,11 +23987,11 @@
     </row>
     <row r="43" spans="1:22" s="7" customFormat="1">
       <c r="A43" s="2" t="s">
-        <v>1360</v>
+        <v>1359</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="D43" s="2"/>
       <c r="F43" s="1"/>
@@ -23946,11 +24012,11 @@
     </row>
     <row r="44" spans="1:22" s="7" customFormat="1">
       <c r="A44" s="2" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
-        <v>1361</v>
+        <v>1360</v>
       </c>
       <c r="D44" s="2"/>
       <c r="F44" s="1"/>
@@ -23971,11 +24037,11 @@
     </row>
     <row r="45" spans="1:22" s="7" customFormat="1">
       <c r="A45" s="2" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="D45" s="2"/>
       <c r="F45" s="1"/>
@@ -23996,11 +24062,11 @@
     </row>
     <row r="46" spans="1:22" s="7" customFormat="1">
       <c r="A46" s="2" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="D46" s="2"/>
       <c r="F46" s="1"/>
@@ -24021,11 +24087,11 @@
     </row>
     <row r="47" spans="1:22" s="7" customFormat="1">
       <c r="A47" s="2" t="s">
-        <v>1368</v>
+        <v>1367</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="D47" s="2"/>
       <c r="F47" s="1"/>
@@ -24046,12 +24112,12 @@
     </row>
     <row r="48" spans="1:22" s="7" customFormat="1" ht="28.8">
       <c r="A48" s="49" t="s">
-        <v>1432</v>
+        <v>1430</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="2"/>
@@ -24073,7 +24139,7 @@
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
-        <v>1435</v>
+        <v>1433</v>
       </c>
       <c r="D49" s="2"/>
       <c r="F49" s="1"/>
@@ -24096,7 +24162,7 @@
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2" t="s">
-        <v>1433</v>
+        <v>1431</v>
       </c>
       <c r="D50" s="2"/>
       <c r="F50" s="1"/>
@@ -24119,7 +24185,7 @@
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
       <c r="D51" s="2"/>
       <c r="F51" s="1"/>
@@ -24142,7 +24208,7 @@
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2" t="s">
-        <v>1436</v>
+        <v>1434</v>
       </c>
       <c r="D52" s="2"/>
       <c r="F52" s="1"/>
@@ -24164,7 +24230,7 @@
     <row r="53" spans="1:22" s="7" customFormat="1" ht="43.2">
       <c r="A53" s="2"/>
       <c r="B53" s="117" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -24186,12 +24252,12 @@
     </row>
     <row r="54" spans="1:22" s="7" customFormat="1" ht="28.8">
       <c r="A54" s="57" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="2"/>
@@ -24213,7 +24279,7 @@
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="D55" s="2"/>
       <c r="F55" s="1"/>
@@ -24235,10 +24301,10 @@
     <row r="56" spans="1:22" s="7" customFormat="1" ht="187.2">
       <c r="A56" s="2"/>
       <c r="B56" s="115" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="D56" s="2"/>
       <c r="F56" s="1"/>
@@ -24259,16 +24325,16 @@
     </row>
     <row r="57" spans="1:22" s="7" customFormat="1" ht="28.8">
       <c r="A57" s="44" t="s">
+        <v>1390</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>1391</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>1405</v>
-      </c>
-      <c r="C57" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>1392</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>1393</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="2"/>
@@ -24288,16 +24354,16 @@
     </row>
     <row r="58" spans="1:22" s="7" customFormat="1" ht="360">
       <c r="A58" s="115" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>1394</v>
+        <v>1516</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>1426</v>
+        <v>1424</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>1395</v>
+        <v>1393</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="2"/>
@@ -24319,7 +24385,7 @@
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
       <c r="D59" s="2"/>
       <c r="F59" s="1"/>
@@ -24340,7 +24406,7 @@
     </row>
     <row r="60" spans="1:22" s="7" customFormat="1">
       <c r="A60" s="2" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -24365,7 +24431,7 @@
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="D61" s="2"/>
       <c r="F61" s="1"/>
@@ -24386,7 +24452,7 @@
     </row>
     <row r="62" spans="1:22" s="7" customFormat="1">
       <c r="A62" s="49" t="s">
-        <v>1396</v>
+        <v>1394</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -24409,11 +24475,11 @@
     </row>
     <row r="63" spans="1:22" s="7" customFormat="1">
       <c r="A63" s="2" t="s">
-        <v>1397</v>
+        <v>1395</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="2" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
       <c r="D63" s="2"/>
       <c r="F63" s="1"/>
@@ -24434,11 +24500,11 @@
     </row>
     <row r="64" spans="1:22" s="7" customFormat="1">
       <c r="A64" s="2" t="s">
-        <v>1398</v>
+        <v>1396</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2" t="s">
-        <v>1402</v>
+        <v>1400</v>
       </c>
       <c r="D64" s="2"/>
       <c r="F64" s="1"/>
@@ -24459,11 +24525,11 @@
     </row>
     <row r="65" spans="1:22" s="7" customFormat="1">
       <c r="A65" s="2" t="s">
-        <v>1399</v>
+        <v>1397</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="2" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
       <c r="D65" s="2"/>
       <c r="F65" s="1"/>
@@ -24484,11 +24550,11 @@
     </row>
     <row r="66" spans="1:22" s="7" customFormat="1">
       <c r="A66" s="2" t="s">
-        <v>1400</v>
+        <v>1398</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" s="2" t="s">
-        <v>1404</v>
+        <v>1402</v>
       </c>
       <c r="D66" s="2"/>
       <c r="F66" s="1"/>
@@ -24510,10 +24576,10 @@
     <row r="67" spans="1:22" s="7" customFormat="1" ht="345.6">
       <c r="A67" s="2"/>
       <c r="B67" s="2" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>1428</v>
+        <v>1426</v>
       </c>
       <c r="D67" s="2"/>
       <c r="F67" s="1"/>
@@ -24536,10 +24602,10 @@
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="2"/>
@@ -24563,10 +24629,10 @@
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
       <c r="F69" s="1"/>
       <c r="G69" s="2"/>
@@ -24588,7 +24654,7 @@
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="D70" s="2"/>
       <c r="F70" s="1"/>
@@ -24609,7 +24675,7 @@
     </row>
     <row r="71" spans="1:22" s="7" customFormat="1">
       <c r="A71" s="44" t="s">
-        <v>1421</v>
+        <v>1419</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -24634,10 +24700,10 @@
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>1425</v>
+        <v>1423</v>
       </c>
       <c r="F72" s="1"/>
       <c r="G72" s="2"/>
@@ -24657,7 +24723,7 @@
     </row>
     <row r="73" spans="1:22" s="7" customFormat="1">
       <c r="A73" s="44" t="s">
-        <v>1422</v>
+        <v>1420</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -24682,7 +24748,7 @@
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2" t="s">
-        <v>1416</v>
+        <v>1414</v>
       </c>
       <c r="D74" s="2"/>
       <c r="F74" s="1"/>
@@ -24703,7 +24769,7 @@
     </row>
     <row r="75" spans="1:22" s="7" customFormat="1">
       <c r="A75" s="44" t="s">
-        <v>1418</v>
+        <v>1416</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -24728,7 +24794,7 @@
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2" t="s">
-        <v>1417</v>
+        <v>1415</v>
       </c>
       <c r="D76" s="2"/>
       <c r="F76" s="1"/>
@@ -24749,7 +24815,7 @@
     </row>
     <row r="77" spans="1:22" s="7" customFormat="1">
       <c r="A77" s="104" t="s">
-        <v>1419</v>
+        <v>1417</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -24774,7 +24840,7 @@
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2" t="s">
-        <v>1420</v>
+        <v>1418</v>
       </c>
       <c r="D78" s="2"/>
       <c r="F78" s="1"/>
@@ -24795,7 +24861,7 @@
     </row>
     <row r="79" spans="1:22" s="7" customFormat="1">
       <c r="A79" s="104" t="s">
-        <v>1424</v>
+        <v>1422</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -24820,7 +24886,7 @@
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2" t="s">
-        <v>1423</v>
+        <v>1421</v>
       </c>
       <c r="D80" s="2"/>
       <c r="F80" s="1"/>
@@ -24846,7 +24912,7 @@
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
       <c r="F81" s="1"/>
       <c r="G81" s="2"/>
@@ -24868,7 +24934,7 @@
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="D82" s="2"/>
       <c r="F82" s="1"/>
@@ -24891,7 +24957,7 @@
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
       <c r="D83" s="2"/>
       <c r="F83" s="1"/>
@@ -24912,7 +24978,7 @@
     </row>
     <row r="84" spans="1:22" s="7" customFormat="1">
       <c r="A84" s="45" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -24937,7 +25003,7 @@
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="D85" s="2"/>
       <c r="F85" s="1"/>
@@ -24960,7 +25026,7 @@
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="D86" s="2"/>
       <c r="F86" s="1"/>
@@ -24983,7 +25049,7 @@
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="D87" s="2"/>
       <c r="F87" s="1"/>
@@ -25003,7 +25069,7 @@
       <c r="V87" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="15" type="noConversion"/>
+  <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="10" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -25076,10 +25142,10 @@
         <v>301</v>
       </c>
       <c r="C3" s="116" t="s">
+        <v>1377</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>1378</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>1379</v>
       </c>
       <c r="P3" s="1"/>
       <c r="U3" s="1"/>
@@ -25087,33 +25153,33 @@
     </row>
     <row r="4" spans="1:22">
       <c r="A4" s="12" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="57.6">
       <c r="C5" s="115" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="158.4">
       <c r="C7" s="115" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="244.8">
       <c r="B8" s="2" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="C8" s="115" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="9" spans="1:22" ht="187.2">
       <c r="B9" s="2" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="C9" s="115" t="s">
-        <v>1384</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="10" spans="1:22">
@@ -25121,33 +25187,33 @@
         <v>753</v>
       </c>
       <c r="C10" s="115" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="11" spans="1:22">
       <c r="A11" s="1" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="C11" s="115" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="28.8">
       <c r="A12" s="1" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="C12" s="115" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="14" spans="1:22">
       <c r="A14" s="12" t="s">
-        <v>1461</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" ht="331.2">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="316.8">
       <c r="C15" s="115" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
     </row>
   </sheetData>
@@ -25164,8 +25230,8 @@
   </sheetPr>
   <dimension ref="A2:V13"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -25223,10 +25289,10 @@
         <v>301</v>
       </c>
       <c r="C3" s="116" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="P3" s="1"/>
       <c r="U3" s="1"/>
@@ -25234,12 +25300,12 @@
     </row>
     <row r="4" spans="1:22">
       <c r="A4" s="12" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="72">
       <c r="C5" s="115" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="6" spans="1:22">
@@ -25247,57 +25313,60 @@
         <v>754</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="7" spans="1:22">
       <c r="A7" s="1" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
       <c r="C7" s="115" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="8" spans="1:22">
       <c r="A8" s="1" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="C8" s="115" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="9" spans="1:22">
       <c r="A9" s="1" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
       <c r="C9" s="115" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="10" spans="1:22">
       <c r="A10" s="1" t="s">
+        <v>1452</v>
+      </c>
+      <c r="C10" s="115" t="s">
         <v>1454</v>
-      </c>
-      <c r="C10" s="115" t="s">
-        <v>1456</v>
       </c>
     </row>
     <row r="11" spans="1:22">
       <c r="A11" s="1" t="s">
+        <v>1453</v>
+      </c>
+      <c r="C11" s="115" t="s">
         <v>1455</v>
-      </c>
-      <c r="C11" s="115" t="s">
-        <v>1457</v>
       </c>
     </row>
     <row r="12" spans="1:22">
       <c r="A12" s="13" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="331.2">
-      <c r="C13" s="115" t="s">
-        <v>1463</v>
+      <c r="B13" s="2" t="s">
+        <v>1514</v>
+      </c>
+      <c r="C13" s="120" t="s">
+        <v>1461</v>
       </c>
     </row>
   </sheetData>
@@ -25314,7 +25383,7 @@
   </sheetPr>
   <dimension ref="A2:V12"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B14" sqref="B12:B14"/>
     </sheetView>
   </sheetViews>
@@ -25373,10 +25442,10 @@
         <v>301</v>
       </c>
       <c r="C3" s="116" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
       <c r="P3" s="1"/>
       <c r="U3" s="1"/>
@@ -25389,48 +25458,48 @@
     </row>
     <row r="5" spans="1:22">
       <c r="C5" s="115" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="28.8">
       <c r="C6" s="115" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="172.8">
       <c r="C7" s="115" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="403.2">
       <c r="B8" s="2" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
       <c r="C8" s="115" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="9" spans="1:22">
       <c r="A9" s="12" t="s">
+        <v>1468</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>1470</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>1472</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="28.8">
       <c r="C10" s="115" t="s">
-        <v>1473</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="28.8">
       <c r="C11" s="115" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="409.6">
       <c r="C12" s="115" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
     </row>
   </sheetData>
@@ -25567,7 +25636,7 @@
   </sheetPr>
   <dimension ref="A2:V40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -25626,7 +25695,7 @@
         <v>301</v>
       </c>
       <c r="C3" s="116" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
       <c r="P3" s="1"/>
       <c r="U3" s="1"/>
@@ -25634,15 +25703,15 @@
     </row>
     <row r="4" spans="1:22">
       <c r="C4" s="115" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="5" spans="1:22">
       <c r="C5" s="115" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="6" spans="1:22">
@@ -25657,67 +25726,67 @@
     </row>
     <row r="8" spans="1:22">
       <c r="C8" s="115" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="9" spans="1:22">
       <c r="C9" s="115" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1505</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="10" spans="1:22">
       <c r="C10" s="115" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="11" spans="1:22">
       <c r="C11" s="115" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="13" spans="1:22">
       <c r="A13" s="118" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="28.8">
       <c r="C14" s="115" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="302.39999999999998">
       <c r="C15" s="115" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="16" spans="1:22">
       <c r="A16" s="12" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>1485</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="C17" s="115" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="331.2">
       <c r="B18" s="2" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
       <c r="C18" s="115" t="s">
-        <v>1489</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -25725,22 +25794,22 @@
         <v>1308</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="28.8">
       <c r="C20" s="115" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="302.39999999999998">
       <c r="C21" s="115" t="s">
-        <v>1493</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="172.8">
       <c r="C22" s="115" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -25750,75 +25819,75 @@
     </row>
     <row r="24" spans="1:4" ht="409.6">
       <c r="B24" s="2" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
       <c r="C24" s="115" t="s">
-        <v>1495</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="12" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>1499</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="129.6">
       <c r="B26" s="2" t="s">
-        <v>1502</v>
+        <v>1500</v>
       </c>
       <c r="C26" s="115" t="s">
-        <v>1497</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="230.4">
       <c r="B27" s="2" t="s">
-        <v>1500</v>
+        <v>1498</v>
       </c>
       <c r="C27" s="115" t="s">
-        <v>1498</v>
+        <v>1496</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>1501</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="12" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>1505</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="28.8">
       <c r="C29" s="115" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="244.8">
       <c r="C30" s="115" t="s">
-        <v>1503</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="12" t="s">
-        <v>1506</v>
+        <v>1504</v>
       </c>
       <c r="C31" s="1"/>
     </row>
     <row r="32" spans="1:4" ht="43.2">
       <c r="A32" s="2"/>
       <c r="C32" s="115" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="86.4">
       <c r="A33" s="2" t="s">
-        <v>1514</v>
+        <v>1512</v>
       </c>
       <c r="C33" s="115" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -25832,7 +25901,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="C36" s="115" t="s">
-        <v>1507</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -25842,23 +25911,23 @@
     </row>
     <row r="38" spans="1:3" ht="129.6">
       <c r="C38" s="115" t="s">
-        <v>1509</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="244.8">
       <c r="A39" s="1" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
       <c r="C39" s="115" t="s">
-        <v>1511</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="288">
       <c r="A40" s="1" t="s">
-        <v>1512</v>
+        <v>1510</v>
       </c>
       <c r="C40" s="115" t="s">
-        <v>1508</v>
+        <v>1506</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
save 03 09 2025
</commit_message>
<xml_diff>
--- a/4 четверть_10_JavaScript_MoleculerJS.xlsx
+++ b/4 четверть_10_JavaScript_MoleculerJS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexServHW\Desktop\GB_Developer_Workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F726B8-09FD-4CF4-B953-F218B772E70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB53E08D-344B-4EAF-8166-B75DE7DFDD15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="13" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13875" yWindow="-21720" windowWidth="51840" windowHeight="21120" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="12" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1818" uniqueCount="1517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1821" uniqueCount="1520">
   <si>
     <t>Документация https://moleculer.services/docs/0.14/broker</t>
   </si>
@@ -17274,17 +17274,105 @@
 };</t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Зачем нужен authorization: true или auth: true?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Автоматическая проверка аутентификации перед выполнением action'а без дублирования кода.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Зачем нужен authentication: true или auth: true?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Автоматическая проверка аутентификации перед выполнением action'а без дублирования кода.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Очень важно! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Все action являются асинхронными. Поэтому возможно два варианта обозначения
+1 async actionName
+return {data:data}
+return {error:error}
+2 actionName {
+return Promise.resolve({data:data})
+return Promise.regect({error:error})
+}</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="41">
+  <fonts count="42">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -17913,7 +18001,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -17924,23 +18012,23 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -17958,7 +18046,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -17976,7 +18064,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -17997,7 +18085,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -18018,7 +18106,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -18036,10 +18124,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -18048,28 +18136,28 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="23" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="24" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -18078,49 +18166,49 @@
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="25" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="26" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="23" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="24" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="23" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="24" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="25" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="26" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -18129,7 +18217,7 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -18138,7 +18226,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -18150,7 +18238,7 @@
     <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -18159,22 +18247,22 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -18186,89 +18274,92 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="23" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="16" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="25" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="26" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -19753,7 +19844,7 @@
       <c r="D27" s="4"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="10" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -22861,7 +22952,7 @@
   <dimension ref="A2:V8"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -22982,8 +23073,8 @@
   </sheetPr>
   <dimension ref="A2:V87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView topLeftCell="A54" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -25069,7 +25160,7 @@
       <c r="V87" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="10" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -25211,7 +25302,7 @@
         <v>1459</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="316.8">
+    <row r="15" spans="1:22" ht="331.2">
       <c r="C15" s="115" t="s">
         <v>1458</v>
       </c>
@@ -25384,7 +25475,7 @@
   <dimension ref="A2:V12"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B14" sqref="B12:B14"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -25461,13 +25552,16 @@
         <v>1462</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="28.8">
-      <c r="C6" s="115" t="s">
+    <row r="6" spans="1:22" ht="43.2">
+      <c r="B6" s="121" t="s">
+        <v>1517</v>
+      </c>
+      <c r="C6" s="121" t="s">
         <v>1463</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="172.8">
-      <c r="C7" s="115" t="s">
+      <c r="C7" s="121" t="s">
         <v>1464</v>
       </c>
     </row>
@@ -25492,8 +25586,11 @@
         <v>1471</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="28.8">
-      <c r="C11" s="115" t="s">
+    <row r="11" spans="1:22" ht="43.2">
+      <c r="B11" s="121" t="s">
+        <v>1518</v>
+      </c>
+      <c r="C11" s="121" t="s">
         <v>1472</v>
       </c>
     </row>
@@ -29670,8 +29767,8 @@
   </sheetPr>
   <dimension ref="A2:V80"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -30288,11 +30385,13 @@
       <c r="U24" s="2"/>
       <c r="V24" s="1"/>
     </row>
-    <row r="25" spans="1:22" s="7" customFormat="1" ht="72">
+    <row r="25" spans="1:22" s="7" customFormat="1" ht="129.6">
       <c r="A25" s="64" t="s">
         <v>1050</v>
       </c>
-      <c r="B25" s="2"/>
+      <c r="B25" s="64" t="s">
+        <v>1519</v>
+      </c>
       <c r="C25" s="52" t="s">
         <v>388</v>
       </c>

</xml_diff>